<commit_message>
initial center is random
</commit_message>
<xml_diff>
--- a/data/centers_information.xlsx
+++ b/data/centers_information.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\coding\centers-monitoring\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E10CA97-53A5-4420-B803-DF7A0BCA71F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DDA934-DBFC-402A-807B-949888E477C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30828" yWindow="612" windowWidth="30936" windowHeight="16896" xr2:uid="{56BE1626-B513-488C-AD81-A1932C63AE59}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="95">
   <si>
     <t>Auburn</t>
   </si>
@@ -306,6 +306,21 @@
   </si>
   <si>
     <t>information</t>
+  </si>
+  <si>
+    <t>county</t>
+  </si>
+  <si>
+    <t>King County</t>
+  </si>
+  <si>
+    <t>Snohomish County</t>
+  </si>
+  <si>
+    <t>Kitsap County</t>
+  </si>
+  <si>
+    <t>Pierce County</t>
   </si>
 </sst>
 </file>
@@ -670,22 +685,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19507F74-8939-4CD2-86FF-8F1F36AB31AE}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="45.81640625" customWidth="1"/>
     <col min="2" max="2" width="30.54296875" customWidth="1"/>
     <col min="3" max="3" width="18.26953125" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" customWidth="1"/>
-    <col min="5" max="5" width="95.81640625" style="2" customWidth="1"/>
+    <col min="4" max="5" width="18.453125" customWidth="1"/>
+    <col min="6" max="6" width="95.81640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>85</v>
       </c>
@@ -699,10 +712,13 @@
         <v>88</v>
       </c>
       <c r="E1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -715,11 +731,14 @@
       <c r="D2">
         <v>2003</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -732,12 +751,15 @@
       <c r="D3">
         <v>1995</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" ht="46" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" ht="46" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -750,12 +772,15 @@
       <c r="D4">
         <v>1995</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -768,12 +793,15 @@
       <c r="D5">
         <v>1995</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -786,11 +814,14 @@
       <c r="D6">
         <v>2005</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -803,11 +834,14 @@
       <c r="D7">
         <v>1995</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -820,12 +854,15 @@
       <c r="D8">
         <v>1995</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -838,11 +875,14 @@
       <c r="D9">
         <v>2015</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -855,11 +895,14 @@
       <c r="D10">
         <v>1995</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" t="s">
+        <v>91</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -872,11 +915,14 @@
       <c r="D11">
         <v>2003</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -889,11 +935,14 @@
       <c r="D12">
         <v>1995</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" t="s">
+        <v>94</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="87" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -906,11 +955,14 @@
       <c r="D13">
         <v>1995</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" t="s">
+        <v>92</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -923,11 +975,14 @@
       <c r="D14">
         <v>1995</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -940,11 +995,14 @@
       <c r="D15">
         <v>1995</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" t="s">
+        <v>94</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="87" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -957,11 +1015,14 @@
       <c r="D16">
         <v>1995</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" t="s">
+        <v>91</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -974,11 +1035,14 @@
       <c r="D17">
         <v>2007</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" t="s">
+        <v>91</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="87" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -991,11 +1055,14 @@
       <c r="D18">
         <v>1995</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" t="s">
+        <v>91</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1008,11 +1075,14 @@
       <c r="D19">
         <v>1995</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" t="s">
+        <v>91</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="88" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="88" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1025,11 +1095,14 @@
       <c r="D20">
         <v>1995</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" t="s">
+        <v>91</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1042,11 +1115,14 @@
       <c r="D21">
         <v>1995</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" t="s">
+        <v>91</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1059,11 +1135,14 @@
       <c r="D22">
         <v>1995</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1076,11 +1155,14 @@
       <c r="D23">
         <v>2007</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" t="s">
+        <v>91</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1093,11 +1175,14 @@
       <c r="D24">
         <v>1995</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" t="s">
+        <v>91</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1110,11 +1195,14 @@
       <c r="D25">
         <v>1995</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E25" t="s">
+        <v>91</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="87" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1127,11 +1215,14 @@
       <c r="D26">
         <v>2003</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E26" t="s">
+        <v>93</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="87" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1144,11 +1235,14 @@
       <c r="D27">
         <v>1995</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" t="s">
+        <v>94</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1161,11 +1255,14 @@
       <c r="D28">
         <v>1995</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" t="s">
+        <v>94</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1178,11 +1275,14 @@
       <c r="D29">
         <v>1995</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E29" t="s">
+        <v>91</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1195,11 +1295,14 @@
       <c r="D30">
         <v>2014</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E30" t="s">
+        <v>94</v>
+      </c>
+      <c r="F30" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1212,11 +1315,14 @@
       <c r="D31">
         <v>2002</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E31" t="s">
+        <v>91</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1229,11 +1335,14 @@
       <c r="D32">
         <v>2019</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E32" t="s">
+        <v>92</v>
+      </c>
+      <c r="F32" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1246,11 +1355,14 @@
       <c r="D33">
         <v>2002</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E33" t="s">
+        <v>91</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1263,11 +1375,14 @@
       <c r="D34">
         <v>2002</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E34" t="s">
+        <v>94</v>
+      </c>
+      <c r="F34" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -1280,11 +1395,14 @@
       <c r="D35">
         <v>2002</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E35" t="s">
+        <v>91</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -1297,11 +1415,14 @@
       <c r="D36">
         <v>2002</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="E36" t="s">
+        <v>91</v>
+      </c>
+      <c r="F36" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -1314,11 +1435,14 @@
       <c r="D37">
         <v>2002</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="E37" t="s">
+        <v>94</v>
+      </c>
+      <c r="F37" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" ht="87" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -1331,11 +1455,14 @@
       <c r="D38">
         <v>2002</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="E38" t="s">
+        <v>92</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" ht="87" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -1348,11 +1475,14 @@
       <c r="D39">
         <v>2003</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="E39" t="s">
+        <v>93</v>
+      </c>
+      <c r="F39" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -1365,11 +1495,14 @@
       <c r="D40">
         <v>2016</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="E40" t="s">
+        <v>94</v>
+      </c>
+      <c r="F40" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>83</v>
       </c>
@@ -1382,7 +1515,10 @@
       <c r="D41">
         <v>2023</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="E41" t="s">
+        <v>91</v>
+      </c>
+      <c r="F41" s="2" t="s">
         <v>84</v>
       </c>
     </row>

</xml_diff>